<commit_message>
Updated bill of materials
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17835" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17835"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="50">
   <si>
     <t>Value</t>
   </si>
@@ -142,6 +142,39 @@
   </si>
   <si>
     <t>M5 nylon locknut</t>
+  </si>
+  <si>
+    <t>MCP6001UT-I/OTCT-ND</t>
+  </si>
+  <si>
+    <t>Operational amplifier, surface mount</t>
+  </si>
+  <si>
+    <t>Zener diode for input bias</t>
+  </si>
+  <si>
+    <t>PRT-12807</t>
+  </si>
+  <si>
+    <t>2x3 male header, 0.1" spacing</t>
+  </si>
+  <si>
+    <t>R1/R2 input resistors, 0603 form factor</t>
+  </si>
+  <si>
+    <t>Rf/Rg feedback and gain resistors, 0603 form factor</t>
+  </si>
+  <si>
+    <t>Rz zener diode current limiting resistor, 0603 form factor</t>
+  </si>
+  <si>
+    <t>Amps</t>
+  </si>
+  <si>
+    <t>Zener Diode Current</t>
+  </si>
+  <si>
+    <t>Rz resistance</t>
   </si>
 </sst>
 </file>
@@ -150,7 +183,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="168" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -218,11 +251,11 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -251,16 +284,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -284,7 +317,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="304800" y="1943100"/>
+          <a:off x="1438275" y="2257425"/>
           <a:ext cx="2857500" cy="1905000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -570,16 +603,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33.28515625" customWidth="1"/>
-    <col min="2" max="2" width="53.42578125" customWidth="1"/>
+    <col min="2" max="2" width="67.7109375" customWidth="1"/>
     <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -626,170 +659,154 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" s="7">
-        <v>3.19</v>
+        <v>43</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0.5</v>
       </c>
       <c r="D3" s="5">
         <v>1</v>
       </c>
       <c r="E3" s="7">
-        <f t="shared" ref="E3:E12" si="0">D3*C3</f>
-        <v>3.19</v>
+        <f>D3*C3</f>
+        <v>0.5</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C4" s="7">
-        <v>2.37</v>
+        <v>3.19</v>
       </c>
       <c r="D4" s="5">
         <v>1</v>
       </c>
       <c r="E4" s="7">
-        <f t="shared" si="0"/>
-        <v>2.37</v>
+        <f t="shared" ref="E4:E19" si="0">D4*C4</f>
+        <v>3.19</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C5" s="7">
-        <v>1.8</v>
+        <v>2.37</v>
       </c>
       <c r="D5" s="5">
         <v>1</v>
       </c>
       <c r="E5" s="7">
         <f t="shared" si="0"/>
-        <v>1.8</v>
+        <v>2.37</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
-        <v>760</v>
+      <c r="A6" s="5" t="s">
+        <v>39</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C6" s="7">
-        <v>3</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="D6" s="5">
         <v>1</v>
       </c>
       <c r="E6" s="7">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
-        <v>661</v>
-      </c>
+      <c r="A7" s="5"/>
       <c r="B7" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="7">
-        <v>0.2</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="C7" s="7"/>
       <c r="D7" s="5">
         <v>1</v>
       </c>
       <c r="E7" s="7">
         <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>0</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
-        <v>30</v>
-      </c>
+      <c r="A8" s="5"/>
       <c r="B8" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="7">
-        <v>1</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="C8" s="7"/>
       <c r="D8" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E8" s="7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
-        <v>36</v>
-      </c>
+      <c r="A9" s="5"/>
       <c r="B9" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" s="7">
-        <v>0.25</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="C9" s="7"/>
       <c r="D9" s="5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E9" s="7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="8">
-        <v>10</v>
-      </c>
+      <c r="A10" s="5"/>
       <c r="B10" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" s="7">
-        <v>0.15</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="C10" s="7"/>
       <c r="D10" s="5">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E10" s="7">
         <f t="shared" si="0"/>
-        <v>0.89999999999999991</v>
+        <v>0</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -804,39 +821,176 @@
       <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="5"/>
+      <c r="A12" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="7">
+        <v>1.8</v>
+      </c>
+      <c r="D12" s="5">
+        <v>1</v>
+      </c>
       <c r="E12" s="7">
         <f t="shared" si="0"/>
+        <v>1.8</v>
+      </c>
+      <c r="F12" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="8">
+        <v>760</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="7">
+        <v>3</v>
+      </c>
+      <c r="D13" s="5">
+        <v>1</v>
+      </c>
+      <c r="E13" s="7">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="8">
+        <v>661</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="D14" s="5">
+        <v>1</v>
+      </c>
+      <c r="E14" s="7">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="8">
+        <v>30</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="7">
+        <v>1</v>
+      </c>
+      <c r="D15" s="5">
+        <v>1</v>
+      </c>
+      <c r="E15" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="D16" s="5">
+        <v>4</v>
+      </c>
+      <c r="E16" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="8">
+        <v>10</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" s="7">
+        <v>0.15</v>
+      </c>
+      <c r="D17" s="5">
+        <v>6</v>
+      </c>
+      <c r="E17" s="7">
+        <f t="shared" si="0"/>
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="7">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F12" s="5"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D14" t="s">
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D21" t="s">
         <v>18</v>
       </c>
-      <c r="E14" s="3">
-        <f>SUM(E2:E12)</f>
-        <v>53.41</v>
+      <c r="E21" s="3">
+        <f>SUM(E2:E19)</f>
+        <v>54.199999999999996</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A9" numberStoredAsText="1"/>
+    <ignoredError sqref="A16" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -958,6 +1112,27 @@
       <c r="C6" t="s">
         <v>13</v>
       </c>
+      <c r="H6">
+        <f>(A2-H2)/A7</f>
+        <v>800</v>
+      </c>
+      <c r="I6" t="s">
+        <v>12</v>
+      </c>
+      <c r="J6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" t="s">
+        <v>48</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated BOM and source model
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17835"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17835" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
     <sheet name="Differential Amp" sheetId="2" r:id="rId2"/>
+    <sheet name="Magnet" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="76">
   <si>
     <t>Value</t>
   </si>
@@ -150,24 +151,15 @@
     <t>Operational amplifier, surface mount</t>
   </si>
   <si>
-    <t>Zener diode for input bias</t>
-  </si>
-  <si>
     <t>PRT-12807</t>
   </si>
   <si>
     <t>2x3 male header, 0.1" spacing</t>
   </si>
   <si>
-    <t>R1/R2 input resistors, 0603 form factor</t>
-  </si>
-  <si>
     <t>Rf/Rg feedback and gain resistors, 0603 form factor</t>
   </si>
   <si>
-    <t>Rz zener diode current limiting resistor, 0603 form factor</t>
-  </si>
-  <si>
     <t>Amps</t>
   </si>
   <si>
@@ -175,15 +167,103 @@
   </si>
   <si>
     <t>Rz resistance</t>
+  </si>
+  <si>
+    <t>12 mm M3 socket head screws, pack of 25</t>
+  </si>
+  <si>
+    <t>M3 nylon locknut</t>
+  </si>
+  <si>
+    <t>in</t>
+  </si>
+  <si>
+    <t>Magnet length</t>
+  </si>
+  <si>
+    <t>Distance from Center (in)</t>
+  </si>
+  <si>
+    <t>Distance from Surface (in)</t>
+  </si>
+  <si>
+    <t>Distance from Surface (mm)</t>
+  </si>
+  <si>
+    <t>Field Strength (gauss)</t>
+  </si>
+  <si>
+    <t>Hall Signal (volts)</t>
+  </si>
+  <si>
+    <t>Arduino ADC Counts</t>
+  </si>
+  <si>
+    <t>Filament Diameter (mm)</t>
+  </si>
+  <si>
+    <t>Mechanical Advantage</t>
+  </si>
+  <si>
+    <t>volts</t>
+  </si>
+  <si>
+    <t>Signal Bias</t>
+  </si>
+  <si>
+    <t>Signal Gain</t>
+  </si>
+  <si>
+    <t>Amplifier Signal (volts)</t>
+  </si>
+  <si>
+    <t>ADC Counts per mm</t>
+  </si>
+  <si>
+    <t>mm per ADC Count</t>
+  </si>
+  <si>
+    <t>568-7089-1-ND</t>
+  </si>
+  <si>
+    <t>Zener diode for input bias, 2.7V 1% 5mA</t>
+  </si>
+  <si>
+    <t>P464DBCT-ND</t>
+  </si>
+  <si>
+    <t>P10KDBCT-ND</t>
+  </si>
+  <si>
+    <t>Rz zener diode current limiting resistor, 464 Ohm 0.1% 0603 form factor</t>
+  </si>
+  <si>
+    <t>R1/R2 input resistors, 10 kOhm 0.1% 0603 form factor</t>
+  </si>
+  <si>
+    <t>P39KDBCT-ND</t>
+  </si>
+  <si>
+    <t>WF8-15</t>
+  </si>
+  <si>
+    <t>Spring for roller arm</t>
+  </si>
+  <si>
+    <t>Extrusion Multiplier</t>
+  </si>
+  <si>
+    <t>Slicer Filament Diameter</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="166" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -245,7 +325,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -262,6 +342,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -278,6 +363,1074 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="3.8535309348957672E-2"/>
+          <c:y val="4.1666666666666664E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="poly"/>
+            <c:order val="5"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="0.13308451828136866"/>
+                  <c:y val="-0.15782407407407406"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="0.00E+00" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Magnet!$G$11:$G$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>979</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>763</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>603</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>483</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>386</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>292</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>225</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>175</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>134</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>65</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Magnet!$H$11:$H$21</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>3.2646595991386445</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0122163326155373</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.7597730660924302</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.5073297995693222</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.2548865330462151</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.0024432665231076</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.497556733476892</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.2451134669537844</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.99267020043067833</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.74022693390757044</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="460439872"/>
+        <c:axId val="460440264"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="460439872"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Arduino ADC Counts</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="460440264"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="460440264"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Filament Diameter</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="460439872"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -335,6 +1488,41 @@
         </a:extLst>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -603,10 +1791,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -659,10 +1847,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>42</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>43</v>
       </c>
       <c r="C3" s="6">
         <v>0.5</v>
@@ -692,7 +1880,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="7">
-        <f t="shared" ref="E4:E19" si="0">D4*C4</f>
+        <f t="shared" ref="E4:E21" si="0">D4*C4</f>
         <v>3.19</v>
       </c>
       <c r="F4" s="5" t="s">
@@ -701,183 +1889,199 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>26</v>
+        <v>72</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>27</v>
+        <v>73</v>
       </c>
       <c r="C5" s="7">
-        <v>2.37</v>
+        <v>1.06</v>
       </c>
       <c r="D5" s="5">
         <v>1</v>
       </c>
       <c r="E5" s="7">
         <f t="shared" si="0"/>
-        <v>2.37</v>
+        <v>1.06</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="C6" s="7">
-        <v>0.28999999999999998</v>
+        <v>2.37</v>
       </c>
       <c r="D6" s="5">
         <v>1</v>
       </c>
       <c r="E6" s="7">
         <f t="shared" si="0"/>
-        <v>0.28999999999999998</v>
+        <v>2.37</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
+      <c r="A7" s="5" t="s">
+        <v>39</v>
+      </c>
       <c r="B7" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C7" s="7"/>
+        <v>40</v>
+      </c>
+      <c r="C7" s="7">
+        <v>0.28999999999999998</v>
+      </c>
       <c r="D7" s="5">
         <v>1</v>
       </c>
       <c r="E7" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="F7" s="5" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
+      <c r="A8" s="5" t="s">
+        <v>65</v>
+      </c>
       <c r="B8" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" s="7"/>
+        <v>66</v>
+      </c>
+      <c r="C8" s="7">
+        <v>0.49</v>
+      </c>
       <c r="D8" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E8" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.49</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
+      <c r="A9" s="5" t="s">
+        <v>68</v>
+      </c>
       <c r="B9" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C9" s="7"/>
+        <v>70</v>
+      </c>
+      <c r="C9" s="7">
+        <v>0.63</v>
+      </c>
       <c r="D9" s="5">
         <v>2</v>
       </c>
       <c r="E9" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.26</v>
       </c>
       <c r="F9" s="5" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
+      <c r="A10" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="B10" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="C10" s="7"/>
+        <v>43</v>
+      </c>
+      <c r="C10" s="7">
+        <v>0.63</v>
+      </c>
       <c r="D10" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E10" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.26</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="5"/>
+      <c r="A11" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C11" s="7">
+        <v>0.63</v>
+      </c>
+      <c r="D11" s="5">
+        <v>1</v>
+      </c>
       <c r="E11" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F11" s="5"/>
+        <v>0.63</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C12" s="7">
-        <v>1.8</v>
-      </c>
-      <c r="D12" s="5">
-        <v>1</v>
-      </c>
+      <c r="A12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="5"/>
       <c r="E12" s="7">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="7">
         <v>1.8</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="8">
-        <v>760</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="7">
-        <v>3</v>
       </c>
       <c r="D13" s="5">
         <v>1</v>
       </c>
       <c r="E13" s="7">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>1.8</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
-        <v>661</v>
+        <v>760</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C14" s="7">
-        <v>0.2</v>
+        <v>3</v>
       </c>
       <c r="D14" s="5">
         <v>1</v>
       </c>
       <c r="E14" s="7">
         <f t="shared" si="0"/>
-        <v>0.2</v>
+        <v>3</v>
       </c>
       <c r="F14" s="5" t="s">
         <v>33</v>
@@ -885,41 +2089,41 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
-        <v>30</v>
+        <v>661</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C15" s="7">
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="D15" s="5">
         <v>1</v>
       </c>
       <c r="E15" s="7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.2</v>
       </c>
       <c r="F15" s="5" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="9" t="s">
-        <v>36</v>
+      <c r="A16" s="8">
+        <v>1024</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="C16" s="7">
-        <v>0.25</v>
+        <v>2</v>
       </c>
       <c r="D16" s="5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E16" s="7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F16" s="5" t="s">
         <v>33</v>
@@ -927,60 +2131,112 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
-        <v>10</v>
+        <v>30</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C17" s="7">
-        <v>0.15</v>
+        <v>1</v>
       </c>
       <c r="D17" s="5">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="E17" s="7">
         <f t="shared" si="0"/>
-        <v>0.89999999999999991</v>
+        <v>1</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="5"/>
+      <c r="A18" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="D18" s="5">
+        <v>4</v>
+      </c>
       <c r="E18" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F18" s="5"/>
+        <v>1</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="5"/>
+      <c r="A19" s="8">
+        <v>10</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="7">
+        <v>0.15</v>
+      </c>
+      <c r="D19" s="5">
+        <v>6</v>
+      </c>
       <c r="E19" s="7">
         <f t="shared" si="0"/>
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="8">
+        <v>870</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="D20" s="5">
+        <v>4</v>
+      </c>
+      <c r="E20" s="7">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="7">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F19" s="5"/>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D21" t="s">
+      <c r="F21" s="5"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
         <v>18</v>
       </c>
-      <c r="E21" s="3">
-        <f>SUM(E2:E19)</f>
-        <v>54.199999999999996</v>
+      <c r="E23" s="3">
+        <f>SUM(E2:E21)</f>
+        <v>61.3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A16" numberStoredAsText="1"/>
+    <ignoredError sqref="A18" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -990,7 +2246,7 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1030,7 +2286,7 @@
       </c>
       <c r="H2">
         <f>A4</f>
-        <v>1</v>
+        <v>2.7</v>
       </c>
       <c r="I2" t="s">
         <v>3</v>
@@ -1051,7 +2307,7 @@
       </c>
       <c r="H3">
         <f>A5-A4</f>
-        <v>0.10000000000000009</v>
+        <v>1.2999999999999998</v>
       </c>
       <c r="I3" t="s">
         <v>3</v>
@@ -1062,7 +2318,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1</v>
+        <v>2.7</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
@@ -1072,7 +2328,7 @@
       </c>
       <c r="H4">
         <f>A2/H3</f>
-        <v>49.999999999999957</v>
+        <v>3.8461538461538467</v>
       </c>
       <c r="I4" t="s">
         <v>10</v>
@@ -1083,7 +2339,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>1.1000000000000001</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
@@ -1093,7 +2349,7 @@
       </c>
       <c r="H5">
         <f>A6*H4</f>
-        <v>499999.99999999959</v>
+        <v>38461.538461538468</v>
       </c>
       <c r="I5" t="s">
         <v>12</v>
@@ -1114,13 +2370,13 @@
       </c>
       <c r="H6">
         <f>(A2-H2)/A7</f>
-        <v>800</v>
+        <v>459.99999999999994</v>
       </c>
       <c r="I6" t="s">
         <v>12</v>
       </c>
       <c r="J6" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1128,10 +2384,10 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C7" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1139,4 +2395,658 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:L21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" customWidth="1"/>
+    <col min="3" max="3" width="12.28515625" customWidth="1"/>
+    <col min="11" max="11" width="10" customWidth="1"/>
+    <col min="12" max="12" width="9.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0.25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f>18/18.111</f>
+        <v>0.99387112804373035</v>
+      </c>
+      <c r="C4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2.7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K7" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="K8">
+        <v>1.75</v>
+      </c>
+      <c r="L8">
+        <v>2.85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="I9" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="K9" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="L9" s="10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0.15</v>
+      </c>
+      <c r="B10">
+        <f>A10-$A$3/2</f>
+        <v>2.4999999999999994E-2</v>
+      </c>
+      <c r="C10">
+        <f>B10*25.4</f>
+        <v>0.63499999999999979</v>
+      </c>
+      <c r="D10">
+        <v>3493.1</v>
+      </c>
+      <c r="E10" s="12">
+        <f>MIN(2.5+0.0014*D10,4)</f>
+        <v>4</v>
+      </c>
+      <c r="F10" s="12">
+        <f>(E10-$A$5)*$A$6</f>
+        <v>5.1999999999999993</v>
+      </c>
+      <c r="G10">
+        <f>_xlfn.FLOOR.MATH(F10*1024/5)</f>
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0.2</v>
+      </c>
+      <c r="B11">
+        <f t="shared" ref="B11:B21" si="0">A11-$A$3/2</f>
+        <v>7.5000000000000011E-2</v>
+      </c>
+      <c r="C11">
+        <f t="shared" ref="C11:C21" si="1">B11*25.4</f>
+        <v>1.9050000000000002</v>
+      </c>
+      <c r="D11">
+        <v>997.2</v>
+      </c>
+      <c r="E11" s="12">
+        <f>MIN(2.5+0.0014*D11,4)</f>
+        <v>3.89608</v>
+      </c>
+      <c r="F11" s="12">
+        <f t="shared" ref="F11:F21" si="2">(E11-$A$5)*$A$6</f>
+        <v>4.7843199999999992</v>
+      </c>
+      <c r="G11">
+        <f t="shared" ref="G11:G21" si="3">_xlfn.FLOOR.MATH(F11*1024/5)</f>
+        <v>979</v>
+      </c>
+      <c r="H11" s="12">
+        <f>($C$17-C11)*$A$4 +1.75</f>
+        <v>3.2646595991386445</v>
+      </c>
+      <c r="I11">
+        <f>(G11-G12)/(H11-H12)</f>
+        <v>855.63779527559188</v>
+      </c>
+      <c r="J11">
+        <f>1/I11</f>
+        <v>1.1687188264958663E-3</v>
+      </c>
+      <c r="K11" s="11">
+        <f>($K$8^2-H11^2)/$K$8^2 + 1</f>
+        <v>-1.4801640157544798</v>
+      </c>
+      <c r="L11" s="11">
+        <f>($L$8^2-H11^2)/$L$8^2 + 1</f>
+        <v>0.68784213010180439</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>0.21</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="0"/>
+        <v>8.4999999999999992E-2</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="1"/>
+        <v>2.1589999999999998</v>
+      </c>
+      <c r="D12">
+        <v>808.2</v>
+      </c>
+      <c r="E12" s="12">
+        <f t="shared" ref="E12:E21" si="4">MIN(2.5+0.0014*D12,4)</f>
+        <v>3.6314799999999998</v>
+      </c>
+      <c r="F12" s="12">
+        <f t="shared" si="2"/>
+        <v>3.7259199999999986</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="3"/>
+        <v>763</v>
+      </c>
+      <c r="H12" s="12">
+        <f>($C$17-C12)*$A$4 +1.75</f>
+        <v>3.0122163326155373</v>
+      </c>
+      <c r="I12">
+        <f t="shared" ref="I12:I20" si="5">(G12-G13)/(H12-H13)</f>
+        <v>633.80577427821618</v>
+      </c>
+      <c r="J12">
+        <f t="shared" ref="J12:J20" si="6">1/I12</f>
+        <v>1.5777704157694196E-3</v>
+      </c>
+      <c r="K12" s="11">
+        <f t="shared" ref="K12:L20" si="7">($K$8^2-H12^2)/$K$8^2 + 1</f>
+        <v>-0.96275828064515823</v>
+      </c>
+      <c r="L12" s="11">
+        <f t="shared" ref="L12:L21" si="8">($L$8^2-H12^2)/$L$8^2 + 1</f>
+        <v>0.88292431708515895</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>0.22</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="0"/>
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="1"/>
+        <v>2.4129999999999998</v>
+      </c>
+      <c r="D13">
+        <v>668.7</v>
+      </c>
+      <c r="E13" s="12">
+        <f t="shared" si="4"/>
+        <v>3.4361800000000002</v>
+      </c>
+      <c r="F13" s="12">
+        <f t="shared" si="2"/>
+        <v>2.9447200000000002</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="3"/>
+        <v>603</v>
+      </c>
+      <c r="H13" s="12">
+        <f>($C$17-C13)*$A$4 +1.75</f>
+        <v>2.7597730660924302</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="5"/>
+        <v>475.35433070866048</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="6"/>
+        <v>2.1036938876925668E-3</v>
+      </c>
+      <c r="K13" s="11">
+        <f t="shared" si="7"/>
+        <v>-0.48697057186260029</v>
+      </c>
+      <c r="L13" s="11">
+        <f t="shared" si="8"/>
+        <v>1.0623148813383549</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>0.23</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="0"/>
+        <v>0.10500000000000001</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="1"/>
+        <v>2.6670000000000003</v>
+      </c>
+      <c r="D14">
+        <v>564.5</v>
+      </c>
+      <c r="E14" s="12">
+        <f t="shared" si="4"/>
+        <v>3.2903000000000002</v>
+      </c>
+      <c r="F14" s="12">
+        <f t="shared" si="2"/>
+        <v>2.3612000000000002</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="3"/>
+        <v>483</v>
+      </c>
+      <c r="H14" s="12">
+        <f>($C$17-C14)*$A$4 +1.75</f>
+        <v>2.5073297995693222</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="5"/>
+        <v>384.24475065616855</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="6"/>
+        <v>2.6025079023000736E-3</v>
+      </c>
+      <c r="K14" s="11">
+        <f t="shared" si="7"/>
+        <v>-5.2800889406804163E-2</v>
+      </c>
+      <c r="L14" s="11">
+        <f t="shared" si="8"/>
+        <v>1.2260138228613928</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>0.24</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="0"/>
+        <v>0.11499999999999999</v>
+      </c>
+      <c r="C15">
+        <f t="shared" si="1"/>
+        <v>2.9209999999999998</v>
+      </c>
+      <c r="D15">
+        <v>480</v>
+      </c>
+      <c r="E15" s="12">
+        <f t="shared" si="4"/>
+        <v>3.1720000000000002</v>
+      </c>
+      <c r="F15" s="12">
+        <f t="shared" si="2"/>
+        <v>1.8879999999999999</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="3"/>
+        <v>386</v>
+      </c>
+      <c r="H15" s="12">
+        <f>($C$17-C15)*$A$4 +1.75</f>
+        <v>2.2548865330462151</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="5"/>
+        <v>372.36089238845136</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="6"/>
+        <v>2.6855666651394421E-3</v>
+      </c>
+      <c r="K15" s="11">
+        <f t="shared" si="7"/>
+        <v>0.33975076672222704</v>
+      </c>
+      <c r="L15" s="11">
+        <f t="shared" si="8"/>
+        <v>1.3740211416542716</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>0.25</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="0"/>
+        <v>0.125</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="1"/>
+        <v>3.1749999999999998</v>
+      </c>
+      <c r="D16">
+        <v>398.1</v>
+      </c>
+      <c r="E16" s="12">
+        <f t="shared" si="4"/>
+        <v>3.0573399999999999</v>
+      </c>
+      <c r="F16" s="12">
+        <f t="shared" si="2"/>
+        <v>1.4293599999999991</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="3"/>
+        <v>292</v>
+      </c>
+      <c r="H16" s="12">
+        <f>($C$17-C16)*$A$4 +1.75</f>
+        <v>2.0024432665231076</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="5"/>
+        <v>265.40616797900259</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="6"/>
+        <v>3.7678099481060828E-3</v>
+      </c>
+      <c r="K16" s="11">
+        <f t="shared" si="7"/>
+        <v>0.69068439652449531</v>
+      </c>
+      <c r="L16" s="11">
+        <f t="shared" si="8"/>
+        <v>1.5063368377169919</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>0.26</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="0"/>
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="C17">
+        <f t="shared" si="1"/>
+        <v>3.4289999999999998</v>
+      </c>
+      <c r="D17">
+        <v>339.7</v>
+      </c>
+      <c r="E17" s="12">
+        <f t="shared" si="4"/>
+        <v>2.9755799999999999</v>
+      </c>
+      <c r="F17" s="12">
+        <f t="shared" si="2"/>
+        <v>1.1023199999999989</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="3"/>
+        <v>225</v>
+      </c>
+      <c r="H17" s="12">
+        <f>($C$17-C17)*$A$4 +1.75</f>
+        <v>1.75</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="5"/>
+        <v>198.06430446194187</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="6"/>
+        <v>5.0488653304621598E-3</v>
+      </c>
+      <c r="K17" s="11">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+      <c r="L17" s="11">
+        <f t="shared" si="8"/>
+        <v>1.6229609110495538</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>0.27</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="0"/>
+        <v>0.14500000000000002</v>
+      </c>
+      <c r="C18">
+        <f t="shared" si="1"/>
+        <v>3.6830000000000003</v>
+      </c>
+      <c r="D18">
+        <v>295.8</v>
+      </c>
+      <c r="E18" s="12">
+        <f t="shared" si="4"/>
+        <v>2.91412</v>
+      </c>
+      <c r="F18" s="12">
+        <f t="shared" si="2"/>
+        <v>0.85647999999999946</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="3"/>
+        <v>175</v>
+      </c>
+      <c r="H18" s="12">
+        <f>($C$17-C18)*$A$4 +1.75</f>
+        <v>1.497556733476892</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="5"/>
+        <v>162.41272965879261</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="6"/>
+        <v>6.157152842027014E-3</v>
+      </c>
+      <c r="K18" s="11">
+        <f t="shared" si="7"/>
+        <v>1.2676975771487415</v>
+      </c>
+      <c r="L18" s="11">
+        <f t="shared" si="8"/>
+        <v>1.7238933616519572</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="0"/>
+        <v>0.15500000000000003</v>
+      </c>
+      <c r="C19">
+        <f t="shared" si="1"/>
+        <v>3.9370000000000003</v>
+      </c>
+      <c r="D19">
+        <v>259.8</v>
+      </c>
+      <c r="E19" s="12">
+        <f t="shared" si="4"/>
+        <v>2.8637199999999998</v>
+      </c>
+      <c r="F19" s="12">
+        <f t="shared" si="2"/>
+        <v>0.65487999999999857</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="3"/>
+        <v>134</v>
+      </c>
+      <c r="H19" s="12">
+        <f>($C$17-C19)*$A$4 +1.75</f>
+        <v>1.2451134669537844</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="5"/>
+        <v>146.56758530183808</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="6"/>
+        <v>6.8227909871109759E-3</v>
+      </c>
+      <c r="K19" s="11">
+        <f t="shared" si="7"/>
+        <v>1.493777127970719</v>
+      </c>
+      <c r="L19" s="11">
+        <f t="shared" si="8"/>
+        <v>1.8091341895242015</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="0"/>
+        <v>0.16499999999999998</v>
+      </c>
+      <c r="C20">
+        <f t="shared" si="1"/>
+        <v>4.1909999999999989</v>
+      </c>
+      <c r="D20">
+        <v>228.2</v>
+      </c>
+      <c r="E20" s="12">
+        <f t="shared" si="4"/>
+        <v>2.81948</v>
+      </c>
+      <c r="F20" s="12">
+        <f t="shared" si="2"/>
+        <v>0.47791999999999923</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="3"/>
+        <v>97</v>
+      </c>
+      <c r="H20" s="12">
+        <f>($C$17-C20)*$A$4 +1.75</f>
+        <v>0.99267020043067833</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="5"/>
+        <v>126.76115485564286</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="6"/>
+        <v>7.8888520788471216E-3</v>
+      </c>
+      <c r="K20" s="11">
+        <f t="shared" si="7"/>
+        <v>1.6782386524659321</v>
+      </c>
+      <c r="L20" s="11">
+        <f t="shared" si="8"/>
+        <v>1.8786833946662871</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>0.3</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="0"/>
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="C21">
+        <f t="shared" si="1"/>
+        <v>4.4449999999999994</v>
+      </c>
+      <c r="D21">
+        <v>200.2</v>
+      </c>
+      <c r="E21" s="12">
+        <f t="shared" si="4"/>
+        <v>2.7802799999999999</v>
+      </c>
+      <c r="F21" s="12">
+        <f t="shared" si="2"/>
+        <v>0.32111999999999874</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="3"/>
+        <v>65</v>
+      </c>
+      <c r="H21" s="12">
+        <f>($C$17-C21)*$A$4 +1.75</f>
+        <v>0.74022693390757044</v>
+      </c>
+      <c r="L21" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated BOM, STLs and added PCBs.
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17835" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17835"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="80">
   <si>
     <t>Value</t>
   </si>
@@ -115,24 +115,12 @@
     <t>digikey</t>
   </si>
   <si>
-    <t>D14</t>
-  </si>
-  <si>
-    <t>Magnet for use with hall effect sensor, Pack of 10</t>
-  </si>
-  <si>
     <t>kjmagnetics</t>
   </si>
   <si>
-    <t>55 mm low profile M5 screw, pack of 10</t>
-  </si>
-  <si>
     <t>openbuildspartstore</t>
   </si>
   <si>
-    <t>15 mm low profile M5 screw, individual</t>
-  </si>
-  <si>
     <t>Ball bearing, 5x15x5</t>
   </si>
   <si>
@@ -169,9 +157,6 @@
     <t>Rz resistance</t>
   </si>
   <si>
-    <t>12 mm M3 socket head screws, pack of 25</t>
-  </si>
-  <si>
     <t>M3 nylon locknut</t>
   </si>
   <si>
@@ -244,9 +229,6 @@
     <t>P39KDBCT-ND</t>
   </si>
   <si>
-    <t>WF8-15</t>
-  </si>
-  <si>
     <t>Spring for roller arm</t>
   </si>
   <si>
@@ -254,6 +236,36 @@
   </si>
   <si>
     <t>Slicer Filament Diameter</t>
+  </si>
+  <si>
+    <t>CBSTSR3-6</t>
+  </si>
+  <si>
+    <t>M3 low profile screw for rotary encoder mounting</t>
+  </si>
+  <si>
+    <t>WF6-15</t>
+  </si>
+  <si>
+    <t>MSSFS3-2.5</t>
+  </si>
+  <si>
+    <t>M3 grub screw for shaft collar</t>
+  </si>
+  <si>
+    <t>25 mm low profile M5 screw, for roller arm axle</t>
+  </si>
+  <si>
+    <t>15 mm low profile M5 screw, for bearing axle</t>
+  </si>
+  <si>
+    <t>12 mm M3 socket head screws, pack of 25, for circuit board mounting</t>
+  </si>
+  <si>
+    <t>DH14</t>
+  </si>
+  <si>
+    <t>Magnet for use with hall effect sensor</t>
   </si>
 </sst>
 </file>
@@ -263,7 +275,7 @@
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -346,7 +358,7 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -593,11 +605,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="460439872"/>
-        <c:axId val="460440264"/>
+        <c:axId val="216969872"/>
+        <c:axId val="263628400"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="460439872"/>
+        <c:axId val="216969872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -710,12 +722,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="460440264"/>
+        <c:crossAx val="263628400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="460440264"/>
+        <c:axId val="263628400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -828,7 +840,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="460439872"/>
+        <c:crossAx val="216969872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1791,10 +1803,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1847,10 +1859,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C3" s="6">
         <v>0.5</v>
@@ -1867,376 +1879,439 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="7">
-        <v>3.19</v>
-      </c>
-      <c r="D4" s="5">
-        <v>1</v>
-      </c>
-      <c r="E4" s="7">
-        <f t="shared" ref="E4:E21" si="0">D4*C4</f>
-        <v>3.19</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>25</v>
-      </c>
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="5"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>72</v>
+        <v>23</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>73</v>
+        <v>24</v>
       </c>
       <c r="C5" s="7">
-        <v>1.06</v>
+        <v>3.19</v>
       </c>
       <c r="D5" s="5">
         <v>1</v>
       </c>
       <c r="E5" s="7">
+        <f t="shared" ref="E5:E26" si="0">D5*C5</f>
+        <v>3.19</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="7">
+        <v>1.06</v>
+      </c>
+      <c r="D6" s="5">
+        <v>1</v>
+      </c>
+      <c r="E6" s="7">
         <f t="shared" si="0"/>
         <v>1.06</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F6" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" s="7">
+        <v>3.6</v>
+      </c>
+      <c r="D7" s="5">
+        <v>3</v>
+      </c>
+      <c r="E7" s="7">
+        <f t="shared" si="0"/>
+        <v>10.8</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" s="7">
+        <v>1.78</v>
+      </c>
+      <c r="D8" s="5">
+        <v>2</v>
+      </c>
+      <c r="E8" s="7">
+        <f t="shared" si="0"/>
+        <v>3.56</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B10" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C10" s="7">
         <v>2.37</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D10" s="5">
         <v>1</v>
       </c>
-      <c r="E6" s="7">
+      <c r="E10" s="7">
         <f t="shared" si="0"/>
         <v>2.37</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F10" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7" s="7">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="7">
         <v>0.28999999999999998</v>
       </c>
-      <c r="D7" s="5">
+      <c r="D11" s="5">
         <v>1</v>
       </c>
-      <c r="E7" s="7">
+      <c r="E11" s="7">
         <f t="shared" si="0"/>
         <v>0.28999999999999998</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F11" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C8" s="7">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" s="7">
         <v>0.49</v>
       </c>
-      <c r="D8" s="5">
+      <c r="D12" s="5">
         <v>1</v>
       </c>
-      <c r="E8" s="7">
+      <c r="E12" s="7">
         <f t="shared" si="0"/>
         <v>0.49</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F12" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C9" s="7">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="7">
         <v>0.63</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D13" s="5">
         <v>2</v>
       </c>
-      <c r="E9" s="7">
+      <c r="E13" s="7">
         <f t="shared" si="0"/>
         <v>1.26</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F13" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C10" s="7">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" s="7">
         <v>0.63</v>
       </c>
-      <c r="D10" s="5">
+      <c r="D14" s="5">
         <v>2</v>
       </c>
-      <c r="E10" s="7">
+      <c r="E14" s="7">
         <f t="shared" si="0"/>
         <v>1.26</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F14" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C11" s="7">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="7">
         <v>0.63</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D15" s="5">
         <v>1</v>
       </c>
-      <c r="E11" s="7">
+      <c r="E15" s="7">
         <f t="shared" si="0"/>
         <v>0.63</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F15" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="7">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="5"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C17" s="7">
+        <v>0.23</v>
+      </c>
+      <c r="D17" s="5">
+        <v>1</v>
+      </c>
+      <c r="E17" s="7">
+        <f t="shared" si="0"/>
+        <v>0.23</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="8">
+        <v>20</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C19" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="D19" s="5">
+        <v>1</v>
+      </c>
+      <c r="E19" s="7">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="8">
+        <v>917</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C20" s="7">
+        <v>0.2</v>
+      </c>
+      <c r="D20" s="5">
+        <v>1</v>
+      </c>
+      <c r="E20" s="7">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="8">
+        <v>1024</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C21" s="7">
+        <v>2</v>
+      </c>
+      <c r="D21" s="5">
+        <v>1</v>
+      </c>
+      <c r="E21" s="7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="8">
+        <v>30</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="7">
+        <v>1</v>
+      </c>
+      <c r="D22" s="5">
+        <v>1</v>
+      </c>
+      <c r="E22" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="7">
+        <v>0.25</v>
+      </c>
+      <c r="D23" s="5">
+        <v>4</v>
+      </c>
+      <c r="E23" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="8">
+        <v>10</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" s="7">
+        <v>0.15</v>
+      </c>
+      <c r="D24" s="5">
+        <v>6</v>
+      </c>
+      <c r="E24" s="7">
+        <f t="shared" si="0"/>
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="8">
+        <v>870</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="7">
+        <v>0.1</v>
+      </c>
+      <c r="D25" s="5">
+        <v>4</v>
+      </c>
+      <c r="E25" s="7">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
+      <c r="F25" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F12" s="5"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="7">
-        <v>1.8</v>
-      </c>
-      <c r="D13" s="5">
-        <v>1</v>
-      </c>
-      <c r="E13" s="7">
-        <f t="shared" si="0"/>
-        <v>1.8</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="8">
-        <v>760</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="7">
-        <v>3</v>
-      </c>
-      <c r="D14" s="5">
-        <v>1</v>
-      </c>
-      <c r="E14" s="7">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="8">
-        <v>661</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="7">
-        <v>0.2</v>
-      </c>
-      <c r="D15" s="5">
-        <v>1</v>
-      </c>
-      <c r="E15" s="7">
-        <f t="shared" si="0"/>
-        <v>0.2</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="8">
-        <v>1024</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C16" s="7">
-        <v>2</v>
-      </c>
-      <c r="D16" s="5">
-        <v>1</v>
-      </c>
-      <c r="E16" s="7">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="8">
-        <v>30</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" s="7">
-        <v>1</v>
-      </c>
-      <c r="D17" s="5">
-        <v>1</v>
-      </c>
-      <c r="E17" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" s="7">
-        <v>0.25</v>
-      </c>
-      <c r="D18" s="5">
-        <v>4</v>
-      </c>
-      <c r="E18" s="7">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="8">
-        <v>10</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C19" s="7">
-        <v>0.15</v>
-      </c>
-      <c r="D19" s="5">
-        <v>6</v>
-      </c>
-      <c r="E19" s="7">
-        <f t="shared" si="0"/>
-        <v>0.89999999999999991</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="8">
-        <v>870</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C20" s="7">
-        <v>0.1</v>
-      </c>
-      <c r="D20" s="5">
-        <v>4</v>
-      </c>
-      <c r="E20" s="7">
-        <f t="shared" si="0"/>
-        <v>0.4</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="7">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F21" s="5"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D23" t="s">
+      <c r="F26" s="5"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
         <v>18</v>
       </c>
-      <c r="E23" s="3">
-        <f>SUM(E2:E21)</f>
-        <v>61.3</v>
+      <c r="E28" s="3">
+        <f>SUM(E2:E26)</f>
+        <v>71.29000000000002</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A18" numberStoredAsText="1"/>
+    <ignoredError sqref="A23" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -2376,7 +2451,7 @@
         <v>12</v>
       </c>
       <c r="J6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -2384,10 +2459,10 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C7" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -2401,8 +2476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:L21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K27" sqref="K27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L11" sqref="L11:L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2419,10 +2494,10 @@
         <v>0.25</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -2431,7 +2506,7 @@
         <v>0.99387112804373035</v>
       </c>
       <c r="C4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -2439,10 +2514,10 @@
         <v>2.7</v>
       </c>
       <c r="B5" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C5" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -2450,12 +2525,12 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -2468,40 +2543,40 @@
     </row>
     <row r="9" spans="1:12" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="G9" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="H9" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="C9" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="D9" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="F9" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="H9" s="10" t="s">
-        <v>57</v>
-      </c>
       <c r="I9" s="10" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="K9" s="10" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="L9" s="10" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -2560,7 +2635,7 @@
         <v>979</v>
       </c>
       <c r="H11" s="12">
-        <f>($C$17-C11)*$A$4 +1.75</f>
+        <f t="shared" ref="H11:H21" si="4">($C$17-C11)*$A$4 +1.75</f>
         <v>3.2646595991386445</v>
       </c>
       <c r="I11">
@@ -2572,12 +2647,12 @@
         <v>1.1687188264958663E-3</v>
       </c>
       <c r="K11" s="11">
-        <f>($K$8^2-H11^2)/$K$8^2 + 1</f>
-        <v>-1.4801640157544798</v>
+        <f>$K$8^2/H11^2</f>
+        <v>0.28734277909692302</v>
       </c>
       <c r="L11" s="11">
-        <f>($L$8^2-H11^2)/$L$8^2 + 1</f>
-        <v>0.68784213010180439</v>
+        <f>$L$8^2/H11^2</f>
+        <v>0.76210341982522689</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -2596,7 +2671,7 @@
         <v>808.2</v>
       </c>
       <c r="E12" s="12">
-        <f t="shared" ref="E12:E21" si="4">MIN(2.5+0.0014*D12,4)</f>
+        <f t="shared" ref="E12:E21" si="5">MIN(2.5+0.0014*D12,4)</f>
         <v>3.6314799999999998</v>
       </c>
       <c r="F12" s="12">
@@ -2608,24 +2683,24 @@
         <v>763</v>
       </c>
       <c r="H12" s="12">
-        <f>($C$17-C12)*$A$4 +1.75</f>
+        <f t="shared" si="4"/>
         <v>3.0122163326155373</v>
       </c>
       <c r="I12">
-        <f t="shared" ref="I12:I20" si="5">(G12-G13)/(H12-H13)</f>
+        <f t="shared" ref="I12:I20" si="6">(G12-G13)/(H12-H13)</f>
         <v>633.80577427821618</v>
       </c>
       <c r="J12">
-        <f t="shared" ref="J12:J20" si="6">1/I12</f>
+        <f t="shared" ref="J12:J20" si="7">1/I12</f>
         <v>1.5777704157694196E-3</v>
       </c>
       <c r="K12" s="11">
-        <f t="shared" ref="K12:L20" si="7">($K$8^2-H12^2)/$K$8^2 + 1</f>
-        <v>-0.96275828064515823</v>
+        <f t="shared" ref="K12:K20" si="8">$K$8^2/H12^2</f>
+        <v>0.33752331620595255</v>
       </c>
       <c r="L12" s="11">
-        <f t="shared" ref="L12:L21" si="8">($L$8^2-H12^2)/$L$8^2 + 1</f>
-        <v>0.88292431708515895</v>
+        <f t="shared" ref="L12:L20" si="9">$L$8^2/H12^2</f>
+        <v>0.89519449334950196</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -2644,7 +2719,7 @@
         <v>668.7</v>
       </c>
       <c r="E13" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.4361800000000002</v>
       </c>
       <c r="F13" s="12">
@@ -2656,24 +2731,24 @@
         <v>603</v>
       </c>
       <c r="H13" s="12">
-        <f>($C$17-C13)*$A$4 +1.75</f>
+        <f t="shared" si="4"/>
         <v>2.7597730660924302</v>
       </c>
       <c r="I13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>475.35433070866048</v>
       </c>
       <c r="J13">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.1036938876925668E-3</v>
       </c>
       <c r="K13" s="11">
-        <f t="shared" si="7"/>
-        <v>-0.48697057186260029</v>
+        <f t="shared" si="8"/>
+        <v>0.40209563044851654</v>
       </c>
       <c r="L13" s="11">
-        <f t="shared" si="8"/>
-        <v>1.0623148813383549</v>
+        <f t="shared" si="9"/>
+        <v>1.0664560843487594</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -2692,7 +2767,7 @@
         <v>564.5</v>
       </c>
       <c r="E14" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.2903000000000002</v>
       </c>
       <c r="F14" s="12">
@@ -2704,24 +2779,24 @@
         <v>483</v>
       </c>
       <c r="H14" s="12">
-        <f>($C$17-C14)*$A$4 +1.75</f>
+        <f t="shared" si="4"/>
         <v>2.5073297995693222</v>
       </c>
       <c r="I14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>384.24475065616855</v>
       </c>
       <c r="J14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.6025079023000736E-3</v>
       </c>
       <c r="K14" s="11">
-        <f t="shared" si="7"/>
-        <v>-5.2800889406804163E-2</v>
+        <f t="shared" si="8"/>
+        <v>0.4871393056970903</v>
       </c>
       <c r="L14" s="11">
-        <f t="shared" si="8"/>
-        <v>1.2260138228613928</v>
+        <f t="shared" si="9"/>
+        <v>1.2920127381304869</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -2740,7 +2815,7 @@
         <v>480</v>
       </c>
       <c r="E15" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.1720000000000002</v>
       </c>
       <c r="F15" s="12">
@@ -2752,24 +2827,24 @@
         <v>386</v>
       </c>
       <c r="H15" s="12">
-        <f>($C$17-C15)*$A$4 +1.75</f>
+        <f t="shared" si="4"/>
         <v>2.2548865330462151</v>
       </c>
       <c r="I15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>372.36089238845136</v>
       </c>
       <c r="J15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2.6855666651394421E-3</v>
       </c>
       <c r="K15" s="11">
-        <f t="shared" si="7"/>
-        <v>0.33975076672222704</v>
+        <f t="shared" si="8"/>
+        <v>0.60231920603012978</v>
       </c>
       <c r="L15" s="11">
-        <f t="shared" si="8"/>
-        <v>1.3740211416542716</v>
+        <f t="shared" si="9"/>
+        <v>1.5974980411362383</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -2788,7 +2863,7 @@
         <v>398.1</v>
       </c>
       <c r="E16" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.0573399999999999</v>
       </c>
       <c r="F16" s="12">
@@ -2800,24 +2875,24 @@
         <v>292</v>
       </c>
       <c r="H16" s="12">
-        <f>($C$17-C16)*$A$4 +1.75</f>
+        <f t="shared" si="4"/>
         <v>2.0024432665231076</v>
       </c>
       <c r="I16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>265.40616797900259</v>
       </c>
       <c r="J16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3.7678099481060828E-3</v>
       </c>
       <c r="K16" s="11">
-        <f t="shared" si="7"/>
-        <v>0.69068439652449531</v>
+        <f t="shared" si="8"/>
+        <v>0.76375779632164786</v>
       </c>
       <c r="L16" s="11">
-        <f t="shared" si="8"/>
-        <v>1.5063368377169919</v>
+        <f t="shared" si="9"/>
+        <v>2.02567271857064</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -2836,7 +2911,7 @@
         <v>339.7</v>
       </c>
       <c r="E17" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.9755799999999999</v>
       </c>
       <c r="F17" s="12">
@@ -2848,24 +2923,24 @@
         <v>225</v>
       </c>
       <c r="H17" s="12">
-        <f>($C$17-C17)*$A$4 +1.75</f>
+        <f t="shared" si="4"/>
         <v>1.75</v>
       </c>
       <c r="I17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>198.06430446194187</v>
       </c>
       <c r="J17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>5.0488653304621598E-3</v>
       </c>
       <c r="K17" s="11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>1</v>
       </c>
       <c r="L17" s="11">
-        <f t="shared" si="8"/>
-        <v>1.6229609110495538</v>
+        <f t="shared" si="9"/>
+        <v>2.6522448979591839</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
@@ -2884,7 +2959,7 @@
         <v>295.8</v>
       </c>
       <c r="E18" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.91412</v>
       </c>
       <c r="F18" s="12">
@@ -2896,24 +2971,24 @@
         <v>175</v>
       </c>
       <c r="H18" s="12">
-        <f>($C$17-C18)*$A$4 +1.75</f>
+        <f t="shared" si="4"/>
         <v>1.497556733476892</v>
       </c>
       <c r="I18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>162.41272965879261</v>
       </c>
       <c r="J18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>6.157152842027014E-3</v>
       </c>
       <c r="K18" s="11">
-        <f t="shared" si="7"/>
-        <v>1.2676975771487415</v>
+        <f t="shared" si="8"/>
+        <v>1.3655560446003261</v>
       </c>
       <c r="L18" s="11">
-        <f t="shared" si="8"/>
-        <v>1.7238933616519572</v>
+        <f t="shared" si="9"/>
+        <v>3.6217890521685385</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -2932,7 +3007,7 @@
         <v>259.8</v>
       </c>
       <c r="E19" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.8637199999999998</v>
       </c>
       <c r="F19" s="12">
@@ -2944,24 +3019,24 @@
         <v>134</v>
       </c>
       <c r="H19" s="12">
-        <f>($C$17-C19)*$A$4 +1.75</f>
+        <f t="shared" si="4"/>
         <v>1.2451134669537844</v>
       </c>
       <c r="I19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>146.56758530183808</v>
       </c>
       <c r="J19">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>6.8227909871109759E-3</v>
       </c>
       <c r="K19" s="11">
-        <f t="shared" si="7"/>
-        <v>1.493777127970719</v>
+        <f t="shared" si="8"/>
+        <v>1.9754144967637062</v>
       </c>
       <c r="L19" s="11">
-        <f t="shared" si="8"/>
-        <v>1.8091341895242015</v>
+        <f t="shared" si="9"/>
+        <v>5.2392830203961482</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
@@ -2980,7 +3055,7 @@
         <v>228.2</v>
       </c>
       <c r="E20" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.81948</v>
       </c>
       <c r="F20" s="12">
@@ -2992,24 +3067,24 @@
         <v>97</v>
       </c>
       <c r="H20" s="12">
-        <f>($C$17-C20)*$A$4 +1.75</f>
+        <f t="shared" si="4"/>
         <v>0.99267020043067833</v>
       </c>
       <c r="I20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>126.76115485564286</v>
       </c>
       <c r="J20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>7.8888520788471216E-3</v>
       </c>
       <c r="K20" s="11">
-        <f t="shared" si="7"/>
-        <v>1.6782386524659321</v>
+        <f t="shared" si="8"/>
+        <v>3.1078934982832904</v>
       </c>
       <c r="L20" s="11">
-        <f t="shared" si="8"/>
-        <v>1.8786833946662871</v>
+        <f t="shared" si="9"/>
+        <v>8.2428946742223754</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -3028,7 +3103,7 @@
         <v>200.2</v>
       </c>
       <c r="E21" s="12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.7802799999999999</v>
       </c>
       <c r="F21" s="12">
@@ -3040,7 +3115,7 @@
         <v>65</v>
       </c>
       <c r="H21" s="12">
-        <f>($C$17-C21)*$A$4 +1.75</f>
+        <f t="shared" si="4"/>
         <v>0.74022693390757044</v>
       </c>
       <c r="L21" s="11"/>

</xml_diff>